<commit_message>
fix typo in _raw_data
</commit_message>
<xml_diff>
--- a/_raw_data_sources.xlsx
+++ b/_raw_data_sources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drussel/Dropbox (Facebook)/Facebook Project - Euro SCI/euro_sci_for_github/_raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drussel/Documents/euro_sci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167B4081-BE4A-0647-9B3C-ED4F856FB4A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16A0CFB-505E-1746-90F2-BB36D6A38DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15900" xr2:uid="{A1D73080-1284-4545-89F2-5DE0A15F896E}"/>
+    <workbookView xWindow="1560" yWindow="3180" windowWidth="28800" windowHeight="15900" xr2:uid="{A1D73080-1284-4545-89F2-5DE0A15F896E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -276,9 +276,6 @@
     <t>We use the open data portal data. However, there are a few regions that appear to be missing. So we backfill manually using data from the report appendix, avaliable here: https://ec.europa.eu/commfrontoffice/publicopinion/index.cfm/survey/getsurveydetail/instruments/flash/surveyky/2219</t>
   </si>
   <si>
-    <t>GADM1 NUTS2 SCI Data (Note: in the script _prep_scripts/build_nuts2_nuts2_sci_data.R, we filter to create  "_raw_data/SCI_Nuts2_Nuts2.csv", which we will use for the rest of the paper)</t>
-  </si>
-  <si>
     <t>Social Connectedness data from Facebook</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>Historical Europe Shapefiles</t>
+  </si>
+  <si>
+    <t>GADM1 NUTS2 SCI Data (Note: in the script _prep_scripts/1_setup_map_and_SCI.R, we filter to create  "_raw_data/SCI_Nuts2_Nuts2.csv", which we will use for the rest of the paper)</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="32" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -715,7 +715,7 @@
     </row>
     <row r="3" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -732,19 +732,19 @@
     </row>
     <row r="4" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="D4" s="3">
         <v>44134</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
another update to raw_data list
</commit_message>
<xml_diff>
--- a/_raw_data_sources.xlsx
+++ b/_raw_data_sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drussel/Documents/euro_sci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16A0CFB-505E-1746-90F2-BB36D6A38DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B66E2F-FFE7-394F-9710-F9208A4027E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="3180" windowWidth="28800" windowHeight="15900" xr2:uid="{A1D73080-1284-4545-89F2-5DE0A15F896E}"/>
+    <workbookView xWindow="-33500" yWindow="-7160" windowWidth="28800" windowHeight="15900" xr2:uid="{A1D73080-1284-4545-89F2-5DE0A15F896E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>NUTS 2016 Shapefiles</t>
-  </si>
-  <si>
     <t>eu_map</t>
   </si>
   <si>
@@ -288,7 +285,10 @@
     <t>Historical Europe Shapefiles</t>
   </si>
   <si>
-    <t>GADM1 NUTS2 SCI Data (Note: in the script _prep_scripts/1_setup_map_and_SCI.R, we filter to create  "_raw_data/SCI_Nuts2_Nuts2.csv", which we will use for the rest of the paper)</t>
+    <t>GADM1 NUTS2 SCI Data (Note: in the script "_prep_scripts/1_setup_map_and_SCI.R", we filter to create  "_raw_data/SCI_Nuts2_Nuts2.csv", which we will use for the rest of the paper)</t>
+  </si>
+  <si>
+    <t>NUTS 2016 Shapefiles (Note: these are downloaded in the script "_prep_scripts/1_setup_map_and_SCI.R")</t>
   </si>
 </sst>
 </file>
@@ -667,7 +667,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="32" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -684,13 +684,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -698,357 +698,357 @@
     </row>
     <row r="2" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3">
         <v>43733</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="3">
         <v>43733</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="D4" s="3">
         <v>44134</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3">
         <v>43734</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D6" s="3">
         <v>43734</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D7" s="3">
         <v>43734</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D8" s="3">
         <v>43734</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D9" s="3">
         <v>43734</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D10" s="3">
         <v>43734</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="D11" s="3">
         <v>43734</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D12" s="3">
         <v>43735</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="3">
         <v>43735</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="3">
         <v>43735</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="3">
         <v>43735</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D16" s="3">
         <v>43735</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="D17" s="3">
         <v>43735</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
         <v>65</v>
       </c>
-      <c r="B18" t="s">
-        <v>66</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="3">
         <v>43735</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
         <v>69</v>
       </c>
-      <c r="B19" t="s">
-        <v>70</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D19" s="3">
         <v>43735</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="3">
         <v>43735</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
         <v>75</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="D21" s="3">
         <v>43738</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" t="s">
         <v>79</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="D22" s="3">
         <v>43738</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>